<commit_message>
change:edit english word change:submit new image of head.
update to unity 5.3.4 f2
Signed-off-by: xxp-macbook-pro <54249636@qq.com>
</commit_message>
<xml_diff>
--- a/ExcelConfig/怪物表.xlsx
+++ b/ExcelConfig/怪物表.xlsx
@@ -1,16 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26101"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiexiongping/Documents/github/workdir/ExcelConfig/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="-90" windowWidth="6300" windowHeight="8895" activeTab="1"/>
+    <workbookView xWindow="3860" yWindow="460" windowWidth="19920" windowHeight="12900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="__Base" sheetId="2" r:id="rId1"/>
     <sheet name="MonsterConfig" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -20,7 +30,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="N3" authorId="0" shapeId="0">
+    <comment ref="N3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,30 +61,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="179">
   <si>
     <t>ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>编号</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>类型</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>备注</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>名称</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Int</t>
@@ -84,137 +94,137 @@
   </si>
   <si>
     <t>MonsterConfig</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MonsterConfig</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MonsterConfig.json</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>怪物表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Float</t>
   </si>
   <si>
     <t>资源名称</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>NPC描述</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>兵种类型</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>生命</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>攻击</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>命中率</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>闪避率</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>速度</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>克制关系暴击</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>暴击倍率</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>技能ID</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>掉落方案ID</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>ResName</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Type</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Hp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Damage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Hit</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Dodge</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Speed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CrtPro</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Mult</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SkillID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DropID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Star</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>兵星</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>js_jiuweihu</t>
   </si>
   <si>
     <t>Level</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>等级</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -236,7 +246,7 @@
       </rPr>
       <t>1</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -264,7 +274,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -296,7 +305,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -328,7 +336,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -354,7 +361,7 @@
       </rPr>
       <t>1</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -382,7 +389,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -414,7 +420,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -446,7 +451,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -472,7 +476,7 @@
       </rPr>
       <t>1</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -500,7 +504,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -532,7 +535,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -564,7 +566,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -596,7 +597,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -622,7 +622,7 @@
       </rPr>
       <t>1</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -650,7 +650,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -682,7 +681,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -714,7 +712,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -746,7 +743,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -778,7 +774,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -810,7 +805,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -842,7 +836,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -868,7 +861,7 @@
       </rPr>
       <t>1</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -896,7 +889,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -928,7 +920,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -960,7 +951,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -992,7 +982,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1024,7 +1013,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1056,7 +1044,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1082,7 +1069,7 @@
       </rPr>
       <t>1</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1110,7 +1097,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1142,7 +1128,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1174,7 +1159,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1206,7 +1190,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1238,7 +1221,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1270,7 +1252,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1302,7 +1283,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1334,7 +1314,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1366,7 +1345,6 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -1374,31 +1352,31 @@
   </si>
   <si>
     <t>红孩儿</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>黄袍怪</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>白骨精</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>黄风怪</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>金角</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>银角</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>莲花洞9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1430,7 +1408,7 @@
       </rPr>
       <t>随机</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1462,7 +1440,7 @@
       </rPr>
       <t>随机</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1494,7 +1472,7 @@
       </rPr>
       <t>随机</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1526,7 +1504,7 @@
       </rPr>
       <t>随机</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1558,7 +1536,7 @@
       </rPr>
       <t>随机</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1590,50 +1568,50 @@
       </rPr>
       <t>随机</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>混世小妖</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>白骨精</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>黄袍怪</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>黄风怪</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>金角</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>银角</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>九尾狐</t>
   </si>
   <si>
     <t>红孩儿</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>八戒元神</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>八戒残魂</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>云栈洞jjc1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>云栈洞jjc2</t>
@@ -1649,7 +1627,7 @@
   </si>
   <si>
     <t>黄风岭jjc1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>黄风岭jjc2</t>
@@ -1665,7 +1643,7 @@
   </si>
   <si>
     <t>白骨洞jjc1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>白骨洞jjc2</t>
@@ -1681,7 +1659,7 @@
   </si>
   <si>
     <t>波月洞jjc1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>波月洞jjc2</t>
@@ -1697,7 +1675,7 @@
   </si>
   <si>
     <t>莲花洞jjc1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>莲花洞jjc2</t>
@@ -1716,7 +1694,7 @@
   </si>
   <si>
     <t>火云洞jjc1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>火云洞jjc2</t>
@@ -1738,123 +1716,123 @@
   </si>
   <si>
     <t>洞口小妖</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>花痴</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>杂役</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>守备猪妖</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>尖耳鼠</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>饕餮鼠</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>鼠妖军备</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>拓耳鼠</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>魅惑女子</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>奸佞老者</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>蒙眼老妪</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>复生亡女</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>诈死老翁</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>狼牙</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>持械狼妖</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>洞穴守备</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>护宝狼妖</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>械斗狼妖</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>黄袍精英</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>独角小妖</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>赤角小妖</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>洞穴卫兵</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>独角蛮兵</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>亲卫</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>赤脚幼童</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>肚兜娃</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>乳牙卫兵</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>小角童儿</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>哭闹小童</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>嬉闹亲卫</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>js_baigujing</t>
@@ -1880,25 +1858,33 @@
   <si>
     <t>js_xiaohou</t>
   </si>
+  <si>
+    <t>js_xiaozhu</t>
+  </si>
+  <si>
+    <t>js_shuyao</t>
+  </si>
+  <si>
+    <t>js_langyao</t>
+  </si>
+  <si>
+    <t>js_huangfengguai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>js_laozhu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2031,28 +2017,28 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2363,16 +2349,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2387,7 +2373,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2396,31 +2382,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T307"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C232" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="V250" sqref="V250"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.75" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="10" width="9" style="2" customWidth="1"/>
     <col min="11" max="13" width="9" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.25" style="2" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" style="2" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="10.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2473,7 +2459,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2526,7 +2512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2579,7 +2565,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -2590,7 +2576,7 @@
         <v>136</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="G4" s="3">
         <v>2</v>
@@ -2633,7 +2619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -2644,7 +2630,7 @@
         <v>136</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="G5" s="3">
         <v>2</v>
@@ -2687,7 +2673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
@@ -2698,7 +2684,7 @@
         <v>136</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="G6" s="3">
         <v>2</v>
@@ -2741,7 +2727,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -2752,7 +2738,7 @@
         <v>136</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="G7" s="3">
         <v>2</v>
@@ -2795,7 +2781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>42</v>
       </c>
@@ -2806,7 +2792,7 @@
         <v>136</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="G8" s="3">
         <v>2</v>
@@ -2849,7 +2835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -2860,7 +2846,7 @@
         <v>137</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>178</v>
       </c>
       <c r="G9" s="3">
         <v>2</v>
@@ -2903,7 +2889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -2914,7 +2900,7 @@
         <v>137</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>178</v>
       </c>
       <c r="G10" s="3">
         <v>2</v>
@@ -2957,7 +2943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -2968,7 +2954,7 @@
         <v>137</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>178</v>
       </c>
       <c r="G11" s="3">
         <v>2</v>
@@ -3011,7 +2997,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -3022,7 +3008,7 @@
         <v>137</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>178</v>
       </c>
       <c r="G12" s="3">
         <v>2</v>
@@ -3065,7 +3051,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
@@ -3076,7 +3062,7 @@
         <v>137</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
+        <v>178</v>
       </c>
       <c r="G13" s="3">
         <v>2</v>
@@ -3119,7 +3105,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -3130,7 +3116,7 @@
         <v>137</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>178</v>
       </c>
       <c r="G14" s="3">
         <v>2</v>
@@ -3173,7 +3159,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>43</v>
       </c>
@@ -3184,7 +3170,7 @@
         <v>137</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>178</v>
       </c>
       <c r="G15" s="3">
         <v>2</v>
@@ -3227,7 +3213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>44</v>
       </c>
@@ -3238,7 +3224,7 @@
         <v>138</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G16" s="3">
         <v>2</v>
@@ -3281,7 +3267,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -3292,7 +3278,7 @@
         <v>138</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G17" s="3">
         <v>2</v>
@@ -3335,7 +3321,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
@@ -3346,7 +3332,7 @@
         <v>138</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G18" s="3">
         <v>2</v>
@@ -3389,7 +3375,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -3400,7 +3386,7 @@
         <v>138</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G19" s="3">
         <v>2</v>
@@ -3443,7 +3429,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
@@ -3454,7 +3440,7 @@
         <v>138</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G20" s="3">
         <v>2</v>
@@ -3497,7 +3483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -3508,7 +3494,7 @@
         <v>138</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G21" s="3">
         <v>2</v>
@@ -3551,7 +3537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>44</v>
       </c>
@@ -3562,7 +3548,7 @@
         <v>138</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G22" s="3">
         <v>2</v>
@@ -3605,7 +3591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -3616,7 +3602,7 @@
         <v>138</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G23" s="3">
         <v>2</v>
@@ -3659,7 +3645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -3670,7 +3656,7 @@
         <v>138</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G24" s="3">
         <v>2</v>
@@ -3713,7 +3699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
@@ -3724,7 +3710,7 @@
         <v>138</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G25" s="3">
         <v>2</v>
@@ -3767,7 +3753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -3778,7 +3764,7 @@
         <v>138</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G26" s="3">
         <v>2</v>
@@ -3821,7 +3807,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>44</v>
       </c>
@@ -3832,7 +3818,7 @@
         <v>138</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="G27" s="3">
         <v>2</v>
@@ -3875,7 +3861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
@@ -3886,7 +3872,7 @@
         <v>139</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="G28" s="3">
         <v>2</v>
@@ -3929,7 +3915,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>87</v>
       </c>
@@ -3940,7 +3926,7 @@
         <v>139</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="G29" s="3">
         <v>2</v>
@@ -3983,7 +3969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>87</v>
       </c>
@@ -3994,7 +3980,7 @@
         <v>139</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="G30" s="3">
         <v>2</v>
@@ -4037,7 +4023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>87</v>
       </c>
@@ -4048,7 +4034,7 @@
         <v>139</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="G31" s="3">
         <v>2</v>
@@ -4091,7 +4077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>87</v>
       </c>
@@ -4102,7 +4088,7 @@
         <v>139</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="G32" s="3">
         <v>2</v>
@@ -4145,7 +4131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>45</v>
       </c>
@@ -4156,7 +4142,7 @@
         <v>102</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>39</v>
+        <v>171</v>
       </c>
       <c r="G33" s="3">
         <v>1</v>
@@ -4199,7 +4185,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>46</v>
       </c>
@@ -4210,7 +4196,7 @@
         <v>140</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G34" s="3">
         <v>2</v>
@@ -4253,7 +4239,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -4264,7 +4250,7 @@
         <v>140</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G35" s="3">
         <v>2</v>
@@ -4307,7 +4293,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
@@ -4318,7 +4304,7 @@
         <v>140</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G36" s="3">
         <v>2</v>
@@ -4361,7 +4347,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -4372,7 +4358,7 @@
         <v>140</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G37" s="3">
         <v>2</v>
@@ -4415,7 +4401,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -4426,7 +4412,7 @@
         <v>140</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G38" s="3">
         <v>2</v>
@@ -4469,7 +4455,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -4480,7 +4466,7 @@
         <v>140</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G39" s="3">
         <v>2</v>
@@ -4523,7 +4509,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -4534,7 +4520,7 @@
         <v>140</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G40" s="3">
         <v>2</v>
@@ -4577,7 +4563,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -4588,7 +4574,7 @@
         <v>140</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G41" s="3">
         <v>2</v>
@@ -4631,7 +4617,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
@@ -4642,7 +4628,7 @@
         <v>140</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G42" s="3">
         <v>2</v>
@@ -4685,7 +4671,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>46</v>
       </c>
@@ -4696,7 +4682,7 @@
         <v>140</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="G43" s="3">
         <v>2</v>
@@ -4739,7 +4725,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>47</v>
       </c>
@@ -4793,7 +4779,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
@@ -4847,7 +4833,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
@@ -4901,7 +4887,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>47</v>
       </c>
@@ -4955,7 +4941,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
@@ -5009,7 +4995,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -5063,7 +5049,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>47</v>
       </c>
@@ -5117,7 +5103,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>47</v>
       </c>
@@ -5171,7 +5157,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>47</v>
       </c>
@@ -5225,7 +5211,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>47</v>
       </c>
@@ -5279,7 +5265,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>48</v>
       </c>
@@ -5333,7 +5319,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>48</v>
       </c>
@@ -5387,7 +5373,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>48</v>
       </c>
@@ -5441,7 +5427,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>48</v>
       </c>
@@ -5495,7 +5481,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>48</v>
       </c>
@@ -5549,7 +5535,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>48</v>
       </c>
@@ -5603,7 +5589,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>48</v>
       </c>
@@ -5657,7 +5643,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>88</v>
       </c>
@@ -5711,7 +5697,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>88</v>
       </c>
@@ -5765,7 +5751,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>88</v>
       </c>
@@ -5819,7 +5805,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>88</v>
       </c>
@@ -5873,7 +5859,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>88</v>
       </c>
@@ -5927,7 +5913,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>49</v>
       </c>
@@ -5981,7 +5967,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>50</v>
       </c>
@@ -6035,7 +6021,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>50</v>
       </c>
@@ -6089,7 +6075,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>50</v>
       </c>
@@ -6143,7 +6129,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>50</v>
       </c>
@@ -6197,7 +6183,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>50</v>
       </c>
@@ -6251,7 +6237,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>50</v>
       </c>
@@ -6305,7 +6291,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>50</v>
       </c>
@@ -6359,7 +6345,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
         <v>50</v>
       </c>
@@ -6413,7 +6399,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>51</v>
       </c>
@@ -6467,7 +6453,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -6521,7 +6507,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>51</v>
       </c>
@@ -6575,7 +6561,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
@@ -6629,7 +6615,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -6683,7 +6669,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>51</v>
       </c>
@@ -6737,7 +6723,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>51</v>
       </c>
@@ -6791,7 +6777,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
         <v>51</v>
       </c>
@@ -6845,7 +6831,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>52</v>
       </c>
@@ -6899,7 +6885,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>52</v>
       </c>
@@ -6953,7 +6939,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>52</v>
       </c>
@@ -7007,7 +6993,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>52</v>
       </c>
@@ -7061,7 +7047,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>52</v>
       </c>
@@ -7115,7 +7101,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
         <v>52</v>
       </c>
@@ -7169,7 +7155,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>53</v>
       </c>
@@ -7223,7 +7209,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>53</v>
       </c>
@@ -7277,7 +7263,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>53</v>
       </c>
@@ -7331,7 +7317,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>53</v>
       </c>
@@ -7385,7 +7371,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>53</v>
       </c>
@@ -7439,7 +7425,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>53</v>
       </c>
@@ -7493,7 +7479,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>53</v>
       </c>
@@ -7547,7 +7533,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
         <v>53</v>
       </c>
@@ -7601,7 +7587,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>89</v>
       </c>
@@ -7655,7 +7641,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>89</v>
       </c>
@@ -7709,7 +7695,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>89</v>
       </c>
@@ -7763,7 +7749,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>89</v>
       </c>
@@ -7817,7 +7803,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>89</v>
       </c>
@@ -7871,7 +7857,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
         <v>89</v>
       </c>
@@ -7925,7 +7911,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
         <v>54</v>
       </c>
@@ -7979,7 +7965,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>55</v>
       </c>
@@ -8033,7 +8019,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>55</v>
       </c>
@@ -8087,7 +8073,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>55</v>
       </c>
@@ -8141,7 +8127,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>55</v>
       </c>
@@ -8195,7 +8181,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
         <v>55</v>
       </c>
@@ -8249,7 +8235,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>56</v>
       </c>
@@ -8303,7 +8289,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>56</v>
       </c>
@@ -8357,7 +8343,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>56</v>
       </c>
@@ -8411,7 +8397,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>56</v>
       </c>
@@ -8465,7 +8451,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
         <v>56</v>
       </c>
@@ -8519,7 +8505,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>57</v>
       </c>
@@ -8573,7 +8559,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>57</v>
       </c>
@@ -8627,7 +8613,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>57</v>
       </c>
@@ -8681,7 +8667,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>57</v>
       </c>
@@ -8735,7 +8721,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
         <v>57</v>
       </c>
@@ -8789,7 +8775,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>58</v>
       </c>
@@ -8843,7 +8829,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>58</v>
       </c>
@@ -8897,7 +8883,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>58</v>
       </c>
@@ -8951,7 +8937,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>58</v>
       </c>
@@ -9005,7 +8991,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
         <v>58</v>
       </c>
@@ -9059,7 +9045,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>59</v>
       </c>
@@ -9113,7 +9099,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>59</v>
       </c>
@@ -9167,7 +9153,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>59</v>
       </c>
@@ -9221,7 +9207,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>59</v>
       </c>
@@ -9275,7 +9261,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
         <v>59</v>
       </c>
@@ -9329,7 +9315,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>60</v>
       </c>
@@ -9383,7 +9369,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>60</v>
       </c>
@@ -9437,7 +9423,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>60</v>
       </c>
@@ -9491,7 +9477,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>60</v>
       </c>
@@ -9545,7 +9531,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
         <v>60</v>
       </c>
@@ -9599,7 +9585,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>61</v>
       </c>
@@ -9653,7 +9639,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>61</v>
       </c>
@@ -9707,7 +9693,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>61</v>
       </c>
@@ -9761,7 +9747,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>61</v>
       </c>
@@ -9815,7 +9801,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
         <v>61</v>
       </c>
@@ -9869,7 +9855,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>90</v>
       </c>
@@ -9923,7 +9909,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>90</v>
       </c>
@@ -9977,7 +9963,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>90</v>
       </c>
@@ -10031,7 +10017,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>90</v>
       </c>
@@ -10085,7 +10071,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>90</v>
       </c>
@@ -10139,7 +10125,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="11" t="s">
         <v>90</v>
       </c>
@@ -10193,7 +10179,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="11" t="s">
         <v>62</v>
       </c>
@@ -10247,7 +10233,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>63</v>
       </c>
@@ -10301,7 +10287,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>63</v>
       </c>
@@ -10355,7 +10341,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>63</v>
       </c>
@@ -10409,7 +10395,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="11" t="s">
         <v>63</v>
       </c>
@@ -10463,7 +10449,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>64</v>
       </c>
@@ -10517,7 +10503,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>64</v>
       </c>
@@ -10571,7 +10557,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>64</v>
       </c>
@@ -10625,7 +10611,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="11" t="s">
         <v>64</v>
       </c>
@@ -10679,7 +10665,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>65</v>
       </c>
@@ -10733,7 +10719,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>65</v>
       </c>
@@ -10787,7 +10773,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>65</v>
       </c>
@@ -10841,7 +10827,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>65</v>
       </c>
@@ -10895,7 +10881,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="11" t="s">
         <v>65</v>
       </c>
@@ -10949,7 +10935,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>66</v>
       </c>
@@ -11003,7 +10989,7 @@
         <v>1951</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>66</v>
       </c>
@@ -11057,7 +11043,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>66</v>
       </c>
@@ -11111,7 +11097,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>66</v>
       </c>
@@ -11165,7 +11151,7 @@
         <v>2095</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>66</v>
       </c>
@@ -11219,7 +11205,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>66</v>
       </c>
@@ -11273,7 +11259,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>66</v>
       </c>
@@ -11327,7 +11313,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>66</v>
       </c>
@@ -11381,7 +11367,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>66</v>
       </c>
@@ -11435,7 +11421,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>66</v>
       </c>
@@ -11489,7 +11475,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>66</v>
       </c>
@@ -11543,7 +11529,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="11" t="s">
         <v>66</v>
       </c>
@@ -11597,7 +11583,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>67</v>
       </c>
@@ -11651,7 +11637,7 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>67</v>
       </c>
@@ -11705,7 +11691,7 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>67</v>
       </c>
@@ -11759,7 +11745,7 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>67</v>
       </c>
@@ -11813,7 +11799,7 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
         <v>67</v>
       </c>
@@ -11867,7 +11853,7 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>68</v>
       </c>
@@ -11921,7 +11907,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>68</v>
       </c>
@@ -11975,7 +11961,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>68</v>
       </c>
@@ -12029,7 +12015,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>68</v>
       </c>
@@ -12083,7 +12069,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>68</v>
       </c>
@@ -12137,7 +12123,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>68</v>
       </c>
@@ -12191,7 +12177,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>68</v>
       </c>
@@ -12245,7 +12231,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="11" t="s">
         <v>68</v>
       </c>
@@ -12299,7 +12285,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="11" t="s">
         <v>68</v>
       </c>
@@ -12353,7 +12339,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>92</v>
       </c>
@@ -12407,7 +12393,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>92</v>
       </c>
@@ -12461,7 +12447,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>92</v>
       </c>
@@ -12515,7 +12501,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>92</v>
       </c>
@@ -12569,7 +12555,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>92</v>
       </c>
@@ -12623,7 +12609,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>92</v>
       </c>
@@ -12677,7 +12663,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>92</v>
       </c>
@@ -12731,7 +12717,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="11" t="s">
         <v>92</v>
       </c>
@@ -12785,7 +12771,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A193" s="11" t="s">
         <v>69</v>
       </c>
@@ -12839,7 +12825,7 @@
         <v>3475</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A194" s="12" t="s">
         <v>86</v>
       </c>
@@ -12893,7 +12879,7 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>70</v>
       </c>
@@ -12947,7 +12933,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>70</v>
       </c>
@@ -13001,7 +12987,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>70</v>
       </c>
@@ -13055,7 +13041,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>70</v>
       </c>
@@ -13109,7 +13095,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" s="11" t="s">
         <v>70</v>
       </c>
@@ -13163,7 +13149,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>71</v>
       </c>
@@ -13217,7 +13203,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>71</v>
       </c>
@@ -13271,7 +13257,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>71</v>
       </c>
@@ -13325,7 +13311,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>71</v>
       </c>
@@ -13379,7 +13365,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A204" s="11" t="s">
         <v>71</v>
       </c>
@@ -13433,7 +13419,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>72</v>
       </c>
@@ -13487,7 +13473,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>72</v>
       </c>
@@ -13541,7 +13527,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>72</v>
       </c>
@@ -13595,7 +13581,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A208" s="11" t="s">
         <v>72</v>
       </c>
@@ -13649,7 +13635,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
         <v>73</v>
       </c>
@@ -13703,7 +13689,7 @@
         <v>8350</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
         <v>73</v>
       </c>
@@ -13757,7 +13743,7 @@
         <v>8350</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>73</v>
       </c>
@@ -13811,7 +13797,7 @@
         <v>8350</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
         <v>73</v>
       </c>
@@ -13865,7 +13851,7 @@
         <v>8350</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A213" s="11" t="s">
         <v>73</v>
       </c>
@@ -13919,7 +13905,7 @@
         <v>8350</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
         <v>74</v>
       </c>
@@ -13973,7 +13959,7 @@
         <v>8900</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
         <v>74</v>
       </c>
@@ -14027,7 +14013,7 @@
         <v>8900</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
         <v>74</v>
       </c>
@@ -14081,7 +14067,7 @@
         <v>8900</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>74</v>
       </c>
@@ -14135,7 +14121,7 @@
         <v>8900</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A218" s="11" t="s">
         <v>74</v>
       </c>
@@ -14189,7 +14175,7 @@
         <v>8900</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
         <v>75</v>
       </c>
@@ -14243,7 +14229,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
         <v>75</v>
       </c>
@@ -14297,7 +14283,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
         <v>75</v>
       </c>
@@ -14351,7 +14337,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
         <v>75</v>
       </c>
@@ -14405,7 +14391,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A223" s="11" t="s">
         <v>75</v>
       </c>
@@ -14459,7 +14445,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
         <v>76</v>
       </c>
@@ -14513,7 +14499,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
         <v>76</v>
       </c>
@@ -14567,7 +14553,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
         <v>76</v>
       </c>
@@ -14621,7 +14607,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
         <v>76</v>
       </c>
@@ -14675,7 +14661,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A228" s="11" t="s">
         <v>76</v>
       </c>
@@ -14729,7 +14715,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
         <v>77</v>
       </c>
@@ -14783,7 +14769,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
         <v>77</v>
       </c>
@@ -14837,7 +14823,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
         <v>77</v>
       </c>
@@ -14891,7 +14877,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
         <v>77</v>
       </c>
@@ -14945,7 +14931,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A233" s="11" t="s">
         <v>77</v>
       </c>
@@ -14999,7 +14985,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
         <v>78</v>
       </c>
@@ -15053,7 +15039,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
         <v>78</v>
       </c>
@@ -15107,7 +15093,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
         <v>78</v>
       </c>
@@ -15161,7 +15147,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
         <v>78</v>
       </c>
@@ -15215,7 +15201,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A238" s="11" t="s">
         <v>78</v>
       </c>
@@ -15269,7 +15255,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
         <v>91</v>
       </c>
@@ -15323,7 +15309,7 @@
         <v>7050</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
         <v>91</v>
       </c>
@@ -15377,7 +15363,7 @@
         <v>7050</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>91</v>
       </c>
@@ -15431,7 +15417,7 @@
         <v>7050</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
         <v>91</v>
       </c>
@@ -15485,7 +15471,7 @@
         <v>7050</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
         <v>91</v>
       </c>
@@ -15539,7 +15525,7 @@
         <v>7050</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
         <v>91</v>
       </c>
@@ -15593,7 +15579,7 @@
         <v>7050</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
         <v>91</v>
       </c>
@@ -15647,7 +15633,7 @@
         <v>7050</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A246" s="11" t="s">
         <v>91</v>
       </c>
@@ -15701,7 +15687,7 @@
         <v>7050</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A247" s="11" t="s">
         <v>79</v>
       </c>
@@ -15755,7 +15741,7 @@
         <v>10164</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B248" s="2">
         <v>245</v>
       </c>
@@ -15796,7 +15782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B249" s="2">
         <v>246</v>
       </c>
@@ -15837,7 +15823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B250" s="2">
         <v>247</v>
       </c>
@@ -15878,7 +15864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="B251" s="2">
         <v>248</v>
       </c>
@@ -15919,7 +15905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="B252" s="2">
         <v>249</v>
       </c>
@@ -15960,7 +15946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="B253" s="2">
         <v>250</v>
       </c>
@@ -16001,7 +15987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="B254" s="2">
         <v>251</v>
       </c>
@@ -16042,7 +16028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="B255" s="2">
         <v>252</v>
       </c>
@@ -16083,7 +16069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="B256" s="2">
         <v>253</v>
       </c>
@@ -16124,7 +16110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="257" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B257" s="2">
         <v>254</v>
       </c>
@@ -16165,7 +16151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="258" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B258" s="2">
         <v>255</v>
       </c>
@@ -16206,7 +16192,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="259" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B259" s="2">
         <v>256</v>
       </c>
@@ -16247,7 +16233,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="260" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B260" s="2">
         <v>257</v>
       </c>
@@ -16288,7 +16274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="261" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B261" s="2">
         <v>258</v>
       </c>
@@ -16329,7 +16315,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="262" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B262" s="2">
         <v>259</v>
       </c>
@@ -16370,7 +16356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B263" s="2">
         <v>260</v>
       </c>
@@ -16411,7 +16397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="264" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B264" s="2">
         <v>261</v>
       </c>
@@ -16452,7 +16438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="265" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B265" s="2">
         <v>262</v>
       </c>
@@ -16493,7 +16479,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="266" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B266" s="2">
         <v>263</v>
       </c>
@@ -16534,7 +16520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="267" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B267" s="2">
         <v>264</v>
       </c>
@@ -16575,7 +16561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="268" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B268" s="2">
         <v>265</v>
       </c>
@@ -16616,7 +16602,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="269" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B269" s="2">
         <v>266</v>
       </c>
@@ -16657,7 +16643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="270" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B270" s="2">
         <v>267</v>
       </c>
@@ -16698,7 +16684,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="271" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B271" s="2">
         <v>268</v>
       </c>
@@ -16739,7 +16725,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="272" spans="2:16" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:16" ht="17" x14ac:dyDescent="0.25">
       <c r="B272" s="2">
         <v>269</v>
       </c>
@@ -16780,7 +16766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="273" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B273" s="2">
         <v>270</v>
       </c>
@@ -16821,7 +16807,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B274" s="2">
         <v>271</v>
       </c>
@@ -16862,7 +16848,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="275" spans="2:20" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:20" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.25">
       <c r="B275" s="14">
         <v>272</v>
       </c>
@@ -16914,7 +16900,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="276" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B276" s="2">
         <v>273</v>
       </c>
@@ -16965,7 +16951,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="277" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B277" s="2">
         <v>274</v>
       </c>
@@ -17016,7 +17002,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="278" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B278" s="2">
         <v>275</v>
       </c>
@@ -17067,7 +17053,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="279" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B279" s="2">
         <v>276</v>
       </c>
@@ -17118,7 +17104,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="280" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B280" s="2">
         <v>277</v>
       </c>
@@ -17169,7 +17155,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="281" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B281" s="2">
         <v>278</v>
       </c>
@@ -17220,7 +17206,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="282" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B282" s="2">
         <v>279</v>
       </c>
@@ -17271,7 +17257,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="283" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B283" s="2">
         <v>280</v>
       </c>
@@ -17322,7 +17308,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="284" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B284" s="2">
         <v>281</v>
       </c>
@@ -17373,7 +17359,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="285" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B285" s="2">
         <v>282</v>
       </c>
@@ -17424,7 +17410,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="286" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B286" s="2">
         <v>283</v>
       </c>
@@ -17475,7 +17461,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="287" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B287" s="2">
         <v>284</v>
       </c>
@@ -17526,7 +17512,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="288" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B288" s="2">
         <v>285</v>
       </c>
@@ -17577,7 +17563,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="289" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B289" s="2">
         <v>286</v>
       </c>
@@ -17628,7 +17614,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="290" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B290" s="2">
         <v>287</v>
       </c>
@@ -17679,7 +17665,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="291" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B291" s="2">
         <v>288</v>
       </c>
@@ -17730,7 +17716,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="292" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B292" s="2">
         <v>289</v>
       </c>
@@ -17781,7 +17767,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="293" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B293" s="2">
         <v>290</v>
       </c>
@@ -17832,7 +17818,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="294" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B294" s="2">
         <v>291</v>
       </c>
@@ -17883,7 +17869,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="295" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B295" s="2">
         <v>292</v>
       </c>
@@ -17934,7 +17920,7 @@
         <v>4625</v>
       </c>
     </row>
-    <row r="296" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B296" s="2">
         <v>293</v>
       </c>
@@ -17985,7 +17971,7 @@
         <v>4625</v>
       </c>
     </row>
-    <row r="297" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B297" s="2">
         <v>294</v>
       </c>
@@ -18036,7 +18022,7 @@
         <v>5775</v>
       </c>
     </row>
-    <row r="298" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B298" s="2">
         <v>295</v>
       </c>
@@ -18087,7 +18073,7 @@
         <v>5775</v>
       </c>
     </row>
-    <row r="299" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B299" s="2">
         <v>296</v>
       </c>
@@ -18138,7 +18124,7 @@
         <v>7225</v>
       </c>
     </row>
-    <row r="300" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B300" s="2">
         <v>297</v>
       </c>
@@ -18189,7 +18175,7 @@
         <v>8675</v>
       </c>
     </row>
-    <row r="301" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B301" s="2">
         <v>298</v>
       </c>
@@ -18240,7 +18226,7 @@
         <v>16632</v>
       </c>
     </row>
-    <row r="302" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B302" s="2">
         <v>299</v>
       </c>
@@ -18291,7 +18277,7 @@
         <v>18720</v>
       </c>
     </row>
-    <row r="303" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B303" s="2">
         <v>300</v>
       </c>
@@ -18342,7 +18328,7 @@
         <v>20808</v>
       </c>
     </row>
-    <row r="304" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B304" s="2">
         <v>301</v>
       </c>
@@ -18393,7 +18379,7 @@
         <v>24948</v>
       </c>
     </row>
-    <row r="305" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="305" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B305" s="2">
         <v>302</v>
       </c>
@@ -18444,7 +18430,7 @@
         <v>27036</v>
       </c>
     </row>
-    <row r="306" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="306" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B306" s="2">
         <v>303</v>
       </c>
@@ -18495,7 +18481,7 @@
         <v>29124</v>
       </c>
     </row>
-    <row r="307" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:20" ht="17" x14ac:dyDescent="0.25">
       <c r="B307" s="2">
         <v>304</v>
       </c>
@@ -18547,7 +18533,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:S2">
       <formula1>"String,Int,DateTime,Float"</formula1>

</xml_diff>